<commit_message>
Noen nye artefakter, meny og changelog
</commit_message>
<xml_diff>
--- a/CodeSystem-no-basis-family-relation.codesystem.xlsx
+++ b/CodeSystem-no-basis-family-relation.codesystem.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Property</t>
   </si>
@@ -391,7 +391,9 @@
       <c r="A11" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" t="s" s="2">
+        <v>16</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">

</xml_diff>